<commit_message>
First update. Waiting for premission
</commit_message>
<xml_diff>
--- a/Excel Sheets/Table.xlsx
+++ b/Excel Sheets/Table.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Unreal Projects\SHU24.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Unreal Projects\SHU24.github.io\Excel Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43EE048-FF88-4F2E-BE58-DBDEBE641A88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083085ED-9083-405B-BD5C-093DE0108A54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{F7742747-AEFC-48B3-A30C-9644DFD93A47}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{F7742747-AEFC-48B3-A30C-9644DFD93A47}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Graph" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="16">
   <si>
     <t>Stint 1</t>
   </si>
@@ -143,6 +144,1042 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Average lap time</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad1!$I$9:$I$16</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Hamish</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Olaf</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Joe</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Matt B.</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>James</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Ewan</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Matt J.</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Chris</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$J$9:$J$16</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>9.2810185185185183E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.3976851851851838E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4664351851851854E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.4701388888888884E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.517978395061728E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.5982060185185179E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.6484953703703706E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.6792824074074066E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9500-4314-9A87-4D50E4ACAAC8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="1550102800"/>
+        <c:axId val="1610685584"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1550102800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1610685584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1610685584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="mm:ss.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1550102800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="206">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>71436</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafiek 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FE2AA19-48B1-4B8D-AAD5-D04BBC618D45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -442,10 +1479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63EC566A-30F6-4A72-9502-2269D1C92C54}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +1490,7 @@
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -464,12 +1501,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>9.2483796296296313E-4</v>
       </c>
@@ -489,7 +1526,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>9.2826388888888895E-4</v>
       </c>
@@ -497,7 +1534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>9.2879629629629638E-4</v>
       </c>
@@ -505,7 +1542,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>9.3050925925925929E-4</v>
       </c>
@@ -513,7 +1550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>9.2810185185185183E-4</v>
       </c>
@@ -521,73 +1558,123 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>9.3899305555555544E-4</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" s="1">
+        <v>9.2810185185185183E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>9.4054398148148144E-4</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="1">
+        <f>($B$9+$B$10)/2</f>
+        <v>9.3976851851851838E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
-        <f>(B9+B10)/2</f>
+        <f>($B$9+$B$10)/2</f>
         <v>9.3976851851851838E-4</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="1">
+        <v>9.4664351851851854E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="1">
+        <v>9.4701388888888884E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>9.560763888888888E-4</v>
       </c>
       <c r="C13" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="1">
+        <v>9.517978395061728E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>9.6356481481481477E-4</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" s="1">
+        <f>($B$13+$B$14)/2</f>
+        <v>9.5982060185185179E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
-        <f>(B13+B14)/2</f>
+        <f>($B$13+$B$14)/2</f>
         <v>9.5982060185185179E-4</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="1">
+        <v>9.6484953703703706E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="1"/>
+      <c r="I16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="1">
+        <v>9.6792824074074066E-4</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
@@ -721,6 +1808,25 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="I9:J16">
+    <sortCondition ref="J16"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E9DD58D-EDBA-4CC7-BEC3-C335019E2F94}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q35" sqref="Q35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>